<commit_message>
Atualização planilha de tarefas
</commit_message>
<xml_diff>
--- a/Planilha de organização de tarefas_att.xlsx
+++ b/Planilha de organização de tarefas_att.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandro V Vieira\Desktop\clones git\Projeto integrador\DOCUMENTOS\DocumentacaoProjeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58272DDA-D4B6-44C3-95A8-0E5F28ED8F77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC79B678-5C31-4749-B1F0-7007B52621C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
   <si>
     <t>TASK 03</t>
   </si>
@@ -335,15 +335,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -362,14 +353,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3009,8 +3009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF609A8-78B1-4901-B1B0-E5F68A46A5C6}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3026,13 +3026,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
@@ -3041,11 +3041,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3060,18 +3060,18 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="D5" s="22" t="s">
+      <c r="B5" s="21"/>
+      <c r="D5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="G5" s="22" t="s">
+      <c r="E5" s="21"/>
+      <c r="G5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="23"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
@@ -3094,171 +3094,171 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16"/>
-      <c r="B7" s="19"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="19" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="19" t="s">
+      <c r="G7" s="13"/>
+      <c r="H7" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
-      <c r="B8" s="20"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="20"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="20"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="17"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="17"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="17"/>
-      <c r="B9" s="20"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="20"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="20"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="17"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="18"/>
-      <c r="B10" s="21"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="21"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="21"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="18"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="18"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="19"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="19" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="19" t="s">
+      <c r="G11" s="13"/>
+      <c r="H11" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="20"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="20"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="20"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="17"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="17"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="20"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="20"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="20"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="17"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="17"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="21"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="21"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="21"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="18"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="18"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="8"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="13"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="8"/>
-      <c r="D16" s="14"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="14"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="8"/>
-      <c r="D17" s="14"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="14"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="9"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="9"/>
-      <c r="G18" s="15"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="19"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="19" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="19" t="s">
+      <c r="G19" s="13"/>
+      <c r="H19" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="20"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="20"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="20"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="17"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="17"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="20"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="20"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="20"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="17"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="17"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="21"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="21"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="21"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="18"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="18"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="D24" s="22" t="s">
+      <c r="B24" s="21"/>
+      <c r="D24" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="G24" s="22" t="s">
+      <c r="E24" s="21"/>
+      <c r="G24" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="23"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
@@ -3281,143 +3281,188 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="16"/>
-      <c r="B26" s="19"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="19"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="16"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="19"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="16"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="17"/>
-      <c r="B27" s="20"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="20"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="20"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="17"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="17"/>
-      <c r="B28" s="20"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="20"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="17"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="20"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="17"/>
     </row>
     <row r="29" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="18"/>
-      <c r="B29" s="21"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="21"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="21"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="18"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="19"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="19"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="19"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="16"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="16"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="20"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="20"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="20"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="17"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="17"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="17"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="20"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="20"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="20"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="17"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="17"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="17"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="21"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="21"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="21"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="18"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="18"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
-      <c r="B34" s="8"/>
-      <c r="D34" s="13"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="22"/>
       <c r="E34" s="8"/>
-      <c r="G34" s="13"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="8"/>
-      <c r="D35" s="14"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="23"/>
       <c r="E35" s="8"/>
-      <c r="G35" s="14"/>
+      <c r="G35" s="23"/>
       <c r="H35" s="8"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="8"/>
-      <c r="D36" s="14"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="23"/>
       <c r="E36" s="8"/>
-      <c r="G36" s="14"/>
+      <c r="G36" s="23"/>
       <c r="H36" s="8"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="9"/>
-      <c r="D37" s="15"/>
+      <c r="D37" s="24"/>
       <c r="E37" s="9"/>
-      <c r="G37" s="15"/>
+      <c r="G37" s="24"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="19"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="19"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="19"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="16"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="16"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="20"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="20"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="20"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="17"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="17"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="17"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="20"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="20"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="20"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="17"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="17"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="17"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="18"/>
-      <c r="B41" s="21"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="21"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="21"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="18"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="18"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="B1:F2"/>
@@ -3434,39 +3479,6 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3496,24 +3508,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3526,18 +3538,18 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="D5" s="22" t="s">
+      <c r="B5" s="21"/>
+      <c r="D5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="G5" s="22" t="s">
+      <c r="E5" s="21"/>
+      <c r="G5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="23"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
@@ -3560,147 +3572,147 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16"/>
-      <c r="B7" s="19"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="19"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="19"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="16"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
-      <c r="B8" s="20"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="20"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="20"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="17"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="17"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="17"/>
-      <c r="B9" s="20"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="20"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="20"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="17"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="18"/>
-      <c r="B10" s="21"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="21"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="21"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="18"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="18"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="19"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="19"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="19"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="16"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="20"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="20"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="20"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="17"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="17"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="20"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="20"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="20"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="17"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="17"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="21"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="21"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="21"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="18"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="18"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="8"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="8"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="8"/>
-      <c r="D16" s="14"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="8"/>
-      <c r="G16" s="14"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="8"/>
-      <c r="D17" s="14"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="8"/>
-      <c r="G17" s="14"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="9"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="9"/>
-      <c r="G18" s="15"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="19"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="19"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="19"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="16"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="20"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="20"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="20"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="17"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="17"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="20"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="20"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="20"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="17"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="17"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="21"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="21"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="21"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="18"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="18"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="D24" s="22" t="s">
+      <c r="B24" s="21"/>
+      <c r="D24" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="G24" s="22" t="s">
+      <c r="E24" s="21"/>
+      <c r="G24" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="23"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
@@ -3723,151 +3735,151 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="16"/>
-      <c r="B26" s="19"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="19"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="16"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="19"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="16"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="17"/>
-      <c r="B27" s="20"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="20"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="20"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="17"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="17"/>
-      <c r="B28" s="20"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="20"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="17"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="20"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="17"/>
     </row>
     <row r="29" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="18"/>
-      <c r="B29" s="21"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="21"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="21"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="18"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="19"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="19"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="19"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="16"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="16"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="16"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="20"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="20"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="20"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="17"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="17"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="17"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="20"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="20"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="20"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="17"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="17"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="17"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="21"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="21"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="21"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="18"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="18"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="8"/>
-      <c r="D34" s="13"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="8"/>
-      <c r="G34" s="13"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="8"/>
-      <c r="D35" s="14"/>
+      <c r="D35" s="23"/>
       <c r="E35" s="8"/>
-      <c r="G35" s="14"/>
+      <c r="G35" s="23"/>
       <c r="H35" s="8"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="8"/>
-      <c r="D36" s="14"/>
+      <c r="D36" s="23"/>
       <c r="E36" s="8"/>
-      <c r="G36" s="14"/>
+      <c r="G36" s="23"/>
       <c r="H36" s="8"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="9"/>
-      <c r="D37" s="15"/>
+      <c r="D37" s="24"/>
       <c r="E37" s="9"/>
-      <c r="G37" s="15"/>
+      <c r="G37" s="24"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="19"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="19"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="19"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="16"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="16"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="16"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="20"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="20"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="20"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="17"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="17"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="17"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="20"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="20"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="20"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="17"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="17"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="17"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="18"/>
-      <c r="B41" s="21"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="21"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="21"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="18"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="18"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="23"/>
-      <c r="D43" s="22" t="s">
+      <c r="B43" s="21"/>
+      <c r="D43" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="23"/>
+      <c r="E43" s="21"/>
     </row>
     <row r="44" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
@@ -3884,156 +3896,107 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A45" s="16"/>
-      <c r="B45" s="19"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="16"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="19"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="16"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A46" s="17"/>
-      <c r="B46" s="20"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="20"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="17"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A47" s="17"/>
-      <c r="B47" s="20"/>
+      <c r="A47" s="14"/>
+      <c r="B47" s="17"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="20"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="17"/>
     </row>
     <row r="48" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="18"/>
-      <c r="B48" s="21"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="18"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="21"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="18"/>
     </row>
     <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="19"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="19"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="16"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="16"/>
     </row>
     <row r="50" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="20"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="20"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="17"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="17"/>
     </row>
     <row r="51" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="20"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="20"/>
+      <c r="A51" s="14"/>
+      <c r="B51" s="17"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="17"/>
     </row>
     <row r="52" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="18"/>
-      <c r="B52" s="21"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="21"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="18"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="18"/>
     </row>
     <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="13"/>
+      <c r="A53" s="22"/>
       <c r="B53" s="8"/>
-      <c r="D53" s="13"/>
+      <c r="D53" s="22"/>
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="14"/>
+      <c r="A54" s="23"/>
       <c r="B54" s="8"/>
-      <c r="D54" s="14"/>
+      <c r="D54" s="23"/>
       <c r="E54" s="8"/>
     </row>
     <row r="55" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="14"/>
+      <c r="A55" s="23"/>
       <c r="B55" s="8"/>
-      <c r="D55" s="14"/>
+      <c r="D55" s="23"/>
       <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="15"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="9"/>
-      <c r="D56" s="15"/>
+      <c r="D56" s="24"/>
       <c r="E56" s="9"/>
     </row>
     <row r="57" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="19"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="19"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="16"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="16"/>
     </row>
     <row r="58" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="B58" s="20"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="20"/>
+      <c r="A58" s="14"/>
+      <c r="B58" s="17"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="17"/>
     </row>
     <row r="59" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="B59" s="20"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="20"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="17"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="17"/>
     </row>
     <row r="60" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="18"/>
-      <c r="B60" s="21"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="21"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="18"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="H38:H41"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
@@ -4050,6 +4013,55 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Atualizacao planilha de tarefas
</commit_message>
<xml_diff>
--- a/Planilha de organização de tarefas_att.xlsx
+++ b/Planilha de organização de tarefas_att.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandro V Vieira\Desktop\clones git\Projeto integrador\DOCUMENTOS\DocumentacaoProjeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5C5BA5-48B2-4445-8A3E-76B882909C56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A81818-AADB-4E2B-B50F-BD391D56F792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
   </bookViews>
   <sheets>
     <sheet name="Bloco 02" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="25">
   <si>
     <t>TASK 03</t>
   </si>
@@ -335,6 +335,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -353,23 +362,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3009,8 +3009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF609A8-78B1-4901-B1B0-E5F68A46A5C6}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView topLeftCell="A24" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3026,13 +3026,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
@@ -3041,11 +3041,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3060,18 +3060,18 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="23"/>
+      <c r="D5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="G5" s="20" t="s">
+      <c r="E5" s="23"/>
+      <c r="G5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
@@ -3094,171 +3094,171 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="16" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="19"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="16" t="s">
+      <c r="G7" s="16"/>
+      <c r="H7" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="17"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="17"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="20"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="20"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="17"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="17"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="20"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="20"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="15"/>
-      <c r="B10" s="18"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="18"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="18"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="21"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="21"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="16" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="19"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="16" t="s">
+      <c r="G11" s="16"/>
+      <c r="H11" s="19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="17"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="17"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="17"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="20"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="20"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="17"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="17"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="17"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="20"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="20"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="18"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="18"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="18"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="21"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="8"/>
-      <c r="D15" s="22"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="22"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="8"/>
-      <c r="D16" s="23"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="23"/>
+      <c r="G16" s="14"/>
       <c r="H16" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="8"/>
-      <c r="D17" s="23"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="23"/>
+      <c r="G17" s="14"/>
       <c r="H17" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="9"/>
-      <c r="D18" s="24"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="9"/>
-      <c r="G18" s="24"/>
+      <c r="G18" s="15"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="16" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="19"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="16" t="s">
+      <c r="G19" s="16"/>
+      <c r="H19" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="17"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="17"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="17"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="20"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="20"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="17"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="17"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="20"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="20"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="18"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="18"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="18"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="21"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="D24" s="20" t="s">
+      <c r="B24" s="23"/>
+      <c r="D24" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="G24" s="20" t="s">
+      <c r="E24" s="23"/>
+      <c r="G24" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="21"/>
+      <c r="H24" s="23"/>
     </row>
     <row r="25" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
@@ -3281,208 +3281,175 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="13"/>
-      <c r="B26" s="16" t="s">
+      <c r="A26" s="16"/>
+      <c r="B26" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="16" t="s">
+      <c r="D26" s="16"/>
+      <c r="E26" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="16" t="s">
+      <c r="G26" s="16"/>
+      <c r="H26" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
-      <c r="B27" s="17"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="20"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="14"/>
-      <c r="B28" s="17"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="20"/>
     </row>
     <row r="29" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="15"/>
-      <c r="B29" s="18"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="21"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="16" t="s">
+      <c r="A30" s="16"/>
+      <c r="B30" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="16" t="s">
+      <c r="D30" s="16"/>
+      <c r="E30" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G30" s="13"/>
-      <c r="H30" s="16" t="s">
+      <c r="G30" s="16"/>
+      <c r="H30" s="19" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="17"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="17"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="17"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="20"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="20"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="20"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="17"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="17"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="17"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="20"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="20"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="20"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
-      <c r="B33" s="18"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="18"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="18"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="21"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="21"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="22"/>
+      <c r="D34" s="13"/>
       <c r="E34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="22"/>
+      <c r="G34" s="13"/>
       <c r="H34" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="23"/>
+      <c r="D35" s="14"/>
       <c r="E35" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G35" s="23"/>
+      <c r="G35" s="14"/>
       <c r="H35" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="23"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="23"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="8"/>
-      <c r="G36" s="23"/>
+      <c r="G36" s="14"/>
       <c r="H36" s="8"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="9"/>
-      <c r="D37" s="24"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="9"/>
-      <c r="G37" s="24"/>
+      <c r="G37" s="15"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="16" t="s">
+      <c r="A38" s="16"/>
+      <c r="B38" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="16" t="s">
+      <c r="D38" s="16"/>
+      <c r="E38" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G38" s="13"/>
-      <c r="H38" s="16" t="s">
+      <c r="G38" s="16"/>
+      <c r="H38" s="19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="17"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="17"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="17"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="20"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="20"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="20"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="17"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="17"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="17"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="20"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="20"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="20"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
-      <c r="B41" s="18"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="18"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="18"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="21"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="21"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="B1:F2"/>
@@ -3499,6 +3466,39 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3511,8 +3511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327B67CF-FE7D-44E4-A9DC-635976C3C237}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="53" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3528,24 +3528,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3558,18 +3558,18 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="23"/>
+      <c r="D5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="G5" s="20" t="s">
+      <c r="E5" s="23"/>
+      <c r="G5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
@@ -3592,147 +3592,171 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="16"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="16"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="19" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="17"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="17"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="20"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="20"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="17"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="17"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="20"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="20"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="15"/>
-      <c r="B10" s="18"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="18"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="18"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="21"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="21"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="16"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="16"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="19" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="17"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="17"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="17"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="20"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="20"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="17"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="17"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="17"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="20"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="20"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="18"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="18"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="18"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="21"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="8"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="8"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="8"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="8"/>
-      <c r="D16" s="23"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="8"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="14"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="8"/>
-      <c r="D17" s="23"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="8"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="14"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="9"/>
-      <c r="D18" s="24"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="9"/>
-      <c r="G18" s="24"/>
+      <c r="G18" s="15"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="16"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="16"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="17"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="17"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="17"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="20"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="20"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="17"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="17"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="20"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="20"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="18"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="18"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="18"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="21"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="D24" s="20" t="s">
+      <c r="B24" s="23"/>
+      <c r="D24" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="G24" s="20" t="s">
+      <c r="E24" s="23"/>
+      <c r="G24" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="21"/>
+      <c r="H24" s="23"/>
     </row>
     <row r="25" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
@@ -3755,151 +3779,167 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="13"/>
-      <c r="B26" s="16"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="19"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
-      <c r="B27" s="17"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="20"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="14"/>
-      <c r="B28" s="17"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="20"/>
     </row>
     <row r="29" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="15"/>
-      <c r="B29" s="18"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="21"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="16"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="16"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="16"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="16"/>
+      <c r="E30" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" s="19"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="17"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="17"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="17"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="20"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="20"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="20"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="17"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="17"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="17"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="20"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="20"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="20"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
-      <c r="B33" s="18"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="18"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="18"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="21"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="21"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22"/>
-      <c r="B34" s="8"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="8"/>
-      <c r="G34" s="22"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="13"/>
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="8"/>
-      <c r="D35" s="23"/>
+      <c r="D35" s="14"/>
       <c r="E35" s="8"/>
-      <c r="G35" s="23"/>
+      <c r="G35" s="14"/>
       <c r="H35" s="8"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="23"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="8"/>
-      <c r="D36" s="23"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="8"/>
-      <c r="G36" s="23"/>
+      <c r="G36" s="14"/>
       <c r="H36" s="8"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="9"/>
-      <c r="D37" s="24"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="9"/>
-      <c r="G37" s="24"/>
+      <c r="G37" s="15"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="16"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="16"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="16"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="16"/>
+      <c r="E38" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="16"/>
+      <c r="H38" s="19"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="17"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="17"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="17"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="20"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="20"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="20"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="17"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="17"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="17"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="20"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="20"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="20"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
-      <c r="B41" s="18"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="18"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="18"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="21"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="21"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="21"/>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="D43" s="20" t="s">
+      <c r="B43" s="23"/>
+      <c r="D43" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="21"/>
+      <c r="E43" s="23"/>
     </row>
     <row r="44" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
@@ -3916,107 +3956,156 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A45" s="13"/>
-      <c r="B45" s="16"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="19"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A46" s="14"/>
-      <c r="B46" s="17"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="20"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="20"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A47" s="14"/>
-      <c r="B47" s="17"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="20"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="20"/>
     </row>
     <row r="48" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="15"/>
-      <c r="B48" s="18"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="21"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="21"/>
     </row>
     <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="16"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="16"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="19"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="19"/>
     </row>
     <row r="50" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="17"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="17"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="20"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="20"/>
     </row>
     <row r="51" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="17"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="17"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="20"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="20"/>
     </row>
     <row r="52" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="15"/>
-      <c r="B52" s="18"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="18"/>
+      <c r="A52" s="18"/>
+      <c r="B52" s="21"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="21"/>
     </row>
     <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="22"/>
+      <c r="A53" s="13"/>
       <c r="B53" s="8"/>
-      <c r="D53" s="22"/>
+      <c r="D53" s="13"/>
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="23"/>
+      <c r="A54" s="14"/>
       <c r="B54" s="8"/>
-      <c r="D54" s="23"/>
+      <c r="D54" s="14"/>
       <c r="E54" s="8"/>
     </row>
     <row r="55" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="23"/>
+      <c r="A55" s="14"/>
       <c r="B55" s="8"/>
-      <c r="D55" s="23"/>
+      <c r="D55" s="14"/>
       <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="24"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="9"/>
-      <c r="D56" s="24"/>
+      <c r="D56" s="15"/>
       <c r="E56" s="9"/>
     </row>
     <row r="57" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="16"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="16"/>
+      <c r="A57" s="16"/>
+      <c r="B57" s="19"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="19"/>
     </row>
     <row r="58" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="17"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="17"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="20"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="20"/>
     </row>
     <row r="59" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="17"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="17"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="20"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="20"/>
     </row>
     <row r="60" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="15"/>
-      <c r="B60" s="18"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="18"/>
+      <c r="A60" s="18"/>
+      <c r="B60" s="21"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
@@ -4033,55 +4122,6 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>